<commit_message>
version 1.7 (current finished version)
</commit_message>
<xml_diff>
--- a/Homework_5/四元式.xlsx
+++ b/Homework_5/四元式.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20351"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BUAA\大三\编译技术\Homework_5\Homework_5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BUAA\junior\Compiler Tech\Homework_5\Homework_5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08EFE2D0-C39E-4E58-A0C7-AAEDFDE4DE41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2684FA-585A-47B2-8D56-E6333E99EC31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25135" windowHeight="10132" xr2:uid="{A87761FA-A15C-4FFB-88ED-CAD289B72A4C}"/>
+    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13759" xr2:uid="{A87761FA-A15C-4FFB-88ED-CAD289B72A4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="44">
   <si>
     <t>OP</t>
   </si>
@@ -155,6 +154,9 @@
   </si>
   <si>
     <t>call</t>
+  </si>
+  <si>
+    <t>use</t>
   </si>
 </sst>
 </file>
@@ -194,7 +196,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -210,7 +212,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -506,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB3F4561-A320-4CB3-BB52-90C7BB4B527C}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -697,7 +699,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>5</v>
       </c>
@@ -708,7 +710,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>30</v>
       </c>
@@ -716,7 +718,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>21</v>
       </c>
@@ -724,7 +726,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -735,7 +737,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>28</v>
       </c>
@@ -743,7 +745,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -751,7 +753,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>26</v>
       </c>
@@ -759,7 +761,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>21</v>
       </c>
@@ -767,7 +769,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -778,10 +780,13 @@
         <v>35</v>
       </c>
       <c r="D27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -792,7 +797,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -803,24 +808,32 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="C30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
         <v>42</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>